<commit_message>
update append multiple files
</commit_message>
<xml_diff>
--- a/uploads/lieu_followup.xlsx
+++ b/uploads/lieu_followup.xlsx
@@ -1330,8 +1330,10 @@
           <t>Tran Minh Tri10349366</t>
         </is>
       </c>
-      <c r="C69" t="n">
-        <v>4</v>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
       </c>
     </row>
     <row r="70">
@@ -1356,10 +1358,8 @@
           <t>TRAN QUOC VIET10073657</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>117.3</t>
-        </is>
+      <c r="C71" t="n">
+        <v>117.3</v>
       </c>
     </row>
     <row r="72">

</xml_diff>